<commit_message>
fix fb 5, 8, 10, 18
</commit_message>
<xml_diff>
--- a/rtw_excel_report/report_list_price_quotation/list_price_quotation.xlsx
+++ b/rtw_excel_report/report_list_price_quotation/list_price_quotation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\odoo\rtw-custom\rtw_excel_report\report_list_price_quotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08391E47-04C9-401F-9AEB-0C7F5D6CD281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8D324E-E6DF-43CE-9938-76188B7CFD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E293D551-BA95-4F1D-883F-7FB05D66DD4D}"/>
   </bookViews>
@@ -733,8 +733,8 @@
   </sheetPr>
   <dimension ref="A1:G2090"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>